<commit_message>
Ajuste con todos los datos
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\U\SimulacióndeSistemas\TrabajoSDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A842D19-F1B5-4288-B4EF-DB9552C0385F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C2364-A9D1-4CA7-8A92-E1E487882A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempo_entre_llegadas" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -234,7 +234,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -464,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:I168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -477,36 +476,36 @@
     <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -518,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="6">
-        <f>(B2*60)+C2+(D2/1000)</f>
+        <f t="shared" ref="E2:E33" si="0">(B2*60)+C2+(D2/1000)</f>
         <v>3.0089999999999999</v>
       </c>
       <c r="F2" s="8">
@@ -537,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -549,7 +548,7 @@
         <v>33</v>
       </c>
       <c r="E3" s="6">
-        <f>(B3*60)+C3+(D3/1000)</f>
+        <f t="shared" si="0"/>
         <v>42.033000000000001</v>
       </c>
       <c r="F3" s="10"/>
@@ -562,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -574,7 +573,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="6">
-        <f>(B4*60)+C4+(D4/1000)</f>
+        <f t="shared" si="0"/>
         <v>42.023000000000003</v>
       </c>
       <c r="F4" s="10"/>
@@ -587,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -599,12 +598,12 @@
         <v>36</v>
       </c>
       <c r="E5" s="6">
-        <f>(B5*60)+C5+(D5/1000)</f>
+        <f t="shared" si="0"/>
         <v>23.036000000000001</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -616,11 +615,11 @@
         <v>95</v>
       </c>
       <c r="E6" s="6">
-        <f>(B6*60)+C6+(D6/1000)</f>
+        <f t="shared" si="0"/>
         <v>24.094999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -632,11 +631,11 @@
         <v>7</v>
       </c>
       <c r="E7" s="6">
-        <f>(B7*60)+C7+(D7/1000)</f>
+        <f t="shared" si="0"/>
         <v>36.006999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -648,11 +647,11 @@
         <v>39</v>
       </c>
       <c r="E8" s="6">
-        <f>(B8*60)+C8+(D8/1000)</f>
+        <f t="shared" si="0"/>
         <v>16.039000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -664,12 +663,12 @@
         <v>87</v>
       </c>
       <c r="E9" s="6">
-        <f>(B9*60)+C9+(D9/1000)</f>
+        <f t="shared" si="0"/>
         <v>9.0869999999999997</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -681,11 +680,11 @@
         <v>75</v>
       </c>
       <c r="E10" s="6">
-        <f>(B10*60)+C10+(D10/1000)</f>
+        <f t="shared" si="0"/>
         <v>46.075000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -697,11 +696,11 @@
         <v>95</v>
       </c>
       <c r="E11" s="6">
-        <f>(B11*60)+C11+(D11/1000)</f>
+        <f t="shared" si="0"/>
         <v>10.095000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -713,11 +712,11 @@
         <v>19</v>
       </c>
       <c r="E12" s="6">
-        <f>(B12*60)+C12+(D12/1000)</f>
+        <f t="shared" si="0"/>
         <v>19.018999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -729,11 +728,11 @@
         <v>34</v>
       </c>
       <c r="E13" s="6">
-        <f>(B13*60)+C13+(D13/1000)</f>
+        <f t="shared" si="0"/>
         <v>9.0340000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -745,11 +744,11 @@
         <v>94</v>
       </c>
       <c r="E14" s="6">
-        <f>(B14*60)+C14+(D14/1000)</f>
+        <f t="shared" si="0"/>
         <v>12.093999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -761,11 +760,11 @@
         <v>19</v>
       </c>
       <c r="E15" s="6">
-        <f>(B15*60)+C15+(D15/1000)</f>
+        <f t="shared" si="0"/>
         <v>27.018999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -777,11 +776,11 @@
         <v>85</v>
       </c>
       <c r="E16" s="6">
-        <f>(B16*60)+C16+(D16/1000)</f>
+        <f t="shared" si="0"/>
         <v>21.085000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -793,11 +792,11 @@
         <v>87</v>
       </c>
       <c r="E17" s="6">
-        <f>(B17*60)+C17+(D17/1000)</f>
+        <f t="shared" si="0"/>
         <v>13.087</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -809,11 +808,11 @@
         <v>62</v>
       </c>
       <c r="E18" s="6">
-        <f>(B18*60)+C18+(D18/1000)</f>
+        <f t="shared" si="0"/>
         <v>25.062000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -825,11 +824,11 @@
         <v>25</v>
       </c>
       <c r="E19" s="6">
-        <f>(B19*60)+C19+(D19/1000)</f>
+        <f t="shared" si="0"/>
         <v>13.025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -841,11 +840,11 @@
         <v>69</v>
       </c>
       <c r="E20" s="6">
-        <f>(B20*60)+C20+(D20/1000)</f>
+        <f t="shared" si="0"/>
         <v>13.069000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -857,11 +856,11 @@
         <v>96</v>
       </c>
       <c r="E21" s="6">
-        <f>(B21*60)+C21+(D21/1000)</f>
+        <f t="shared" si="0"/>
         <v>28.096</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -873,11 +872,11 @@
         <v>39</v>
       </c>
       <c r="E22" s="6">
-        <f>(B22*60)+C22+(D22/1000)</f>
+        <f t="shared" si="0"/>
         <v>9.0389999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -889,11 +888,11 @@
         <v>21</v>
       </c>
       <c r="E23" s="6">
-        <f>(B23*60)+C23+(D23/1000)</f>
+        <f t="shared" si="0"/>
         <v>8.0210000000000008</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -905,11 +904,11 @@
         <v>2</v>
       </c>
       <c r="E24" s="6">
-        <f>(B24*60)+C24+(D24/1000)</f>
+        <f t="shared" si="0"/>
         <v>47.002000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -921,11 +920,11 @@
         <v>66</v>
       </c>
       <c r="E25" s="6">
-        <f>(B25*60)+C25+(D25/1000)</f>
+        <f t="shared" si="0"/>
         <v>9.0660000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -937,11 +936,11 @@
         <v>88</v>
       </c>
       <c r="E26" s="6">
-        <f>(B26*60)+C26+(D26/1000)</f>
+        <f t="shared" si="0"/>
         <v>35.088000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -953,11 +952,11 @@
         <v>16</v>
       </c>
       <c r="E27" s="6">
-        <f>(B27*60)+C27+(D27/1000)</f>
+        <f t="shared" si="0"/>
         <v>46.015999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -969,11 +968,11 @@
         <v>79</v>
       </c>
       <c r="E28" s="6">
-        <f>(B28*60)+C28+(D28/1000)</f>
+        <f t="shared" si="0"/>
         <v>30.079000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -985,11 +984,11 @@
         <v>97</v>
       </c>
       <c r="E29" s="6">
-        <f>(B29*60)+C29+(D29/1000)</f>
+        <f t="shared" si="0"/>
         <v>15.097</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -1001,11 +1000,11 @@
         <v>4</v>
       </c>
       <c r="E30" s="6">
-        <f>(B30*60)+C30+(D30/1000)</f>
+        <f t="shared" si="0"/>
         <v>13.004</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -1017,11 +1016,11 @@
         <v>99</v>
       </c>
       <c r="E31" s="6">
-        <f>(B31*60)+C31+(D31/1000)</f>
+        <f t="shared" si="0"/>
         <v>14.099</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1033,11 +1032,11 @@
         <v>38</v>
       </c>
       <c r="E32" s="2">
-        <f>(B32*60)+C32+(D32/1000)</f>
+        <f t="shared" si="0"/>
         <v>32.037999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1051,11 +1050,11 @@
         <v>61</v>
       </c>
       <c r="E33" s="2">
-        <f>(B33*60)+C33+(D33/1000)</f>
+        <f t="shared" si="0"/>
         <v>98.061000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1067,11 +1066,11 @@
         <v>34</v>
       </c>
       <c r="E34" s="2">
-        <f>(B34*60)+C34+(D34/1000)</f>
+        <f t="shared" ref="E34:E65" si="1">(B34*60)+C34+(D34/1000)</f>
         <v>5.0339999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1083,11 +1082,11 @@
         <v>68</v>
       </c>
       <c r="E35" s="2">
-        <f>(B35*60)+C35+(D35/1000)</f>
+        <f t="shared" si="1"/>
         <v>24.068000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1101,11 +1100,11 @@
         <v>37</v>
       </c>
       <c r="E36" s="2">
-        <f>(B36*60)+C36+(D36/1000)</f>
+        <f t="shared" si="1"/>
         <v>61.036999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1117,11 +1116,11 @@
         <v>91</v>
       </c>
       <c r="E37" s="2">
-        <f>(B37*60)+C37+(D37/1000)</f>
+        <f t="shared" si="1"/>
         <v>19.091000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1133,11 +1132,11 @@
         <v>8</v>
       </c>
       <c r="E38" s="2">
-        <f>(B38*60)+C38+(D38/1000)</f>
+        <f t="shared" si="1"/>
         <v>28.007999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1149,11 +1148,11 @@
         <v>71</v>
       </c>
       <c r="E39" s="2">
-        <f>(B39*60)+C39+(D39/1000)</f>
+        <f t="shared" si="1"/>
         <v>32.070999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1167,11 +1166,11 @@
         <v>83</v>
       </c>
       <c r="E40" s="2">
-        <f>(B40*60)+C40+(D40/1000)</f>
+        <f t="shared" si="1"/>
         <v>66.082999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1183,11 +1182,11 @@
         <v>67</v>
       </c>
       <c r="E41" s="2">
-        <f>(B41*60)+C41+(D41/1000)</f>
+        <f t="shared" si="1"/>
         <v>52.067</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1201,11 +1200,11 @@
         <v>82</v>
       </c>
       <c r="E42" s="2">
-        <f>(B42*60)+C42+(D42/1000)</f>
+        <f t="shared" si="1"/>
         <v>79.081999999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1217,11 +1216,11 @@
         <v>44</v>
       </c>
       <c r="E43" s="2">
-        <f>(B43*60)+C43+(D43/1000)</f>
+        <f t="shared" si="1"/>
         <v>54.043999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1233,11 +1232,11 @@
         <v>67</v>
       </c>
       <c r="E44" s="2">
-        <f>(B44*60)+C44+(D44/1000)</f>
+        <f t="shared" si="1"/>
         <v>29.067</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1249,11 +1248,11 @@
         <v>19</v>
       </c>
       <c r="E45" s="2">
-        <f>(B45*60)+C45+(D45/1000)</f>
+        <f t="shared" si="1"/>
         <v>8.0190000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1265,11 +1264,11 @@
         <v>14</v>
       </c>
       <c r="E46" s="2">
-        <f>(B46*60)+C46+(D46/1000)</f>
+        <f t="shared" si="1"/>
         <v>27.013999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1281,11 +1280,11 @@
         <v>84</v>
       </c>
       <c r="E47" s="2">
-        <f>(B47*60)+C47+(D47/1000)</f>
+        <f t="shared" si="1"/>
         <v>40.084000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1297,11 +1296,11 @@
         <v>43</v>
       </c>
       <c r="E48" s="2">
-        <f>(B48*60)+C48+(D48/1000)</f>
+        <f t="shared" si="1"/>
         <v>18.042999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1313,11 +1312,11 @@
         <v>8</v>
       </c>
       <c r="E49" s="2">
-        <f>(B49*60)+C49+(D49/1000)</f>
+        <f t="shared" si="1"/>
         <v>41.008000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1329,11 +1328,11 @@
         <v>90</v>
       </c>
       <c r="E50" s="2">
-        <f>(B50*60)+C50+(D50/1000)</f>
+        <f t="shared" si="1"/>
         <v>16.09</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1345,11 +1344,11 @@
         <v>99</v>
       </c>
       <c r="E51" s="2">
-        <f>(B51*60)+C51+(D51/1000)</f>
+        <f t="shared" si="1"/>
         <v>8.0990000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1361,11 +1360,11 @@
         <v>76</v>
       </c>
       <c r="E52" s="2">
-        <f>(B52*60)+C52+(D52/1000)</f>
+        <f t="shared" si="1"/>
         <v>6.0759999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1377,11 +1376,11 @@
         <v>92</v>
       </c>
       <c r="E53" s="2">
-        <f>(B53*60)+C53+(D53/1000)</f>
+        <f t="shared" si="1"/>
         <v>4.0919999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1393,11 +1392,11 @@
         <v>27</v>
       </c>
       <c r="E54" s="2">
-        <f>(B54*60)+C54+(D54/1000)</f>
+        <f t="shared" si="1"/>
         <v>37.027000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1409,11 +1408,11 @@
         <v>33</v>
       </c>
       <c r="E55" s="2">
-        <f>(B55*60)+C55+(D55/1000)</f>
+        <f t="shared" si="1"/>
         <v>11.032999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1425,11 +1424,11 @@
         <v>97</v>
       </c>
       <c r="E56" s="2">
-        <f>(B56*60)+C56+(D56/1000)</f>
+        <f t="shared" si="1"/>
         <v>43.097000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1441,11 +1440,11 @@
         <v>72</v>
       </c>
       <c r="E57" s="2">
-        <f>(B57*60)+C57+(D57/1000)</f>
+        <f t="shared" si="1"/>
         <v>17.071999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1457,11 +1456,11 @@
         <v>57</v>
       </c>
       <c r="E58" s="2">
-        <f>(B58*60)+C58+(D58/1000)</f>
+        <f t="shared" si="1"/>
         <v>8.0570000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1473,11 +1472,11 @@
         <v>82</v>
       </c>
       <c r="E59" s="2">
-        <f>(B59*60)+C59+(D59/1000)</f>
+        <f t="shared" si="1"/>
         <v>39.082000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1489,11 +1488,11 @@
         <v>10</v>
       </c>
       <c r="E60" s="2">
-        <f>(B60*60)+C60+(D60/1000)</f>
+        <f t="shared" si="1"/>
         <v>30.01</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1505,11 +1504,11 @@
         <v>97</v>
       </c>
       <c r="E61" s="2">
-        <f>(B61*60)+C61+(D61/1000)</f>
+        <f t="shared" si="1"/>
         <v>37.097000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1521,11 +1520,11 @@
         <v>30</v>
       </c>
       <c r="E62" s="2">
-        <f>(B62*60)+C62+(D62/1000)</f>
+        <f t="shared" si="1"/>
         <v>23.03</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1537,11 +1536,11 @@
         <v>24</v>
       </c>
       <c r="E63" s="2">
-        <f>(B63*60)+C63+(D63/1000)</f>
+        <f t="shared" si="1"/>
         <v>9.0239999999999991</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1553,11 +1552,11 @@
         <v>65</v>
       </c>
       <c r="E64" s="2">
-        <f>(B64*60)+C64+(D64/1000)</f>
+        <f t="shared" si="1"/>
         <v>39.064999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1569,11 +1568,11 @@
         <v>17</v>
       </c>
       <c r="E65" s="2">
-        <f>(B65*60)+C65+(D65/1000)</f>
+        <f t="shared" si="1"/>
         <v>45.017000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1585,11 +1584,11 @@
         <v>80</v>
       </c>
       <c r="E66" s="2">
-        <f>(B66*60)+C66+(D66/1000)</f>
+        <f t="shared" ref="E66:E97" si="2">(B66*60)+C66+(D66/1000)</f>
         <v>6.08</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1601,11 +1600,11 @@
         <v>50</v>
       </c>
       <c r="E67" s="2">
-        <f>(B67*60)+C67+(D67/1000)</f>
+        <f t="shared" si="2"/>
         <v>31.05</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1617,11 +1616,11 @@
         <v>51</v>
       </c>
       <c r="E68" s="2">
-        <f>(B68*60)+C68+(D68/1000)</f>
+        <f t="shared" si="2"/>
         <v>28.050999999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1633,11 +1632,11 @@
         <v>15</v>
       </c>
       <c r="E69" s="2">
-        <f>(B69*60)+C69+(D69/1000)</f>
+        <f t="shared" si="2"/>
         <v>23.015000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1649,11 +1648,11 @@
         <v>24</v>
       </c>
       <c r="E70" s="2">
-        <f>(B70*60)+C70+(D70/1000)</f>
+        <f t="shared" si="2"/>
         <v>7.024</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1665,11 +1664,11 @@
         <v>73</v>
       </c>
       <c r="E71" s="2">
-        <f>(B71*60)+C71+(D71/1000)</f>
+        <f t="shared" si="2"/>
         <v>20.073</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1683,11 +1682,11 @@
         <v>87</v>
       </c>
       <c r="E72" s="2">
-        <f>(B72*60)+C72+(D72/1000)</f>
+        <f t="shared" si="2"/>
         <v>115.087</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1699,11 +1698,11 @@
         <v>69</v>
       </c>
       <c r="E73" s="2">
-        <f>(B73*60)+C73+(D73/1000)</f>
+        <f t="shared" si="2"/>
         <v>35.069000000000003</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1715,11 +1714,11 @@
         <v>38</v>
       </c>
       <c r="E74" s="2">
-        <f>(B74*60)+C74+(D74/1000)</f>
+        <f t="shared" si="2"/>
         <v>15.038</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1731,11 +1730,11 @@
         <v>85</v>
       </c>
       <c r="E75" s="2">
-        <f>(B75*60)+C75+(D75/1000)</f>
+        <f t="shared" si="2"/>
         <v>26.085000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1747,11 +1746,11 @@
         <v>78</v>
       </c>
       <c r="E76" s="2">
-        <f>(B76*60)+C76+(D76/1000)</f>
+        <f t="shared" si="2"/>
         <v>22.077999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1763,11 +1762,11 @@
         <v>69</v>
       </c>
       <c r="E77" s="2">
-        <f>(B77*60)+C77+(D77/1000)</f>
+        <f t="shared" si="2"/>
         <v>26.068999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -1779,11 +1778,11 @@
         <v>21</v>
       </c>
       <c r="E78" s="2">
-        <f>(B78*60)+C78+(D78/1000)</f>
+        <f t="shared" si="2"/>
         <v>27.021000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -1797,11 +1796,11 @@
         <v>89</v>
       </c>
       <c r="E79" s="2">
-        <f>(B79*60)+C79+(D79/1000)</f>
+        <f t="shared" si="2"/>
         <v>103.089</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -1813,11 +1812,11 @@
         <v>92</v>
       </c>
       <c r="E80" s="2">
-        <f>(B80*60)+C80+(D80/1000)</f>
+        <f t="shared" si="2"/>
         <v>15.092000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -1829,11 +1828,11 @@
         <v>20</v>
       </c>
       <c r="E81" s="2">
-        <f>(B81*60)+C81+(D81/1000)</f>
+        <f t="shared" si="2"/>
         <v>14.02</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -1845,11 +1844,11 @@
         <v>19</v>
       </c>
       <c r="E82" s="2">
-        <f>(B82*60)+C82+(D82/1000)</f>
+        <f t="shared" si="2"/>
         <v>10.019</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -1861,11 +1860,11 @@
         <v>91</v>
       </c>
       <c r="E83" s="2">
-        <f>(B83*60)+C83+(D83/1000)</f>
+        <f t="shared" si="2"/>
         <v>20.091000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -1877,11 +1876,11 @@
         <v>21</v>
       </c>
       <c r="E84" s="2">
-        <f>(B84*60)+C84+(D84/1000)</f>
+        <f t="shared" si="2"/>
         <v>11.021000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -1893,11 +1892,11 @@
         <v>26</v>
       </c>
       <c r="E85" s="2">
-        <f>(B85*60)+C85+(D85/1000)</f>
+        <f t="shared" si="2"/>
         <v>8.0259999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -1909,11 +1908,11 @@
         <v>49</v>
       </c>
       <c r="E86" s="2">
-        <f>(B86*60)+C86+(D86/1000)</f>
+        <f t="shared" si="2"/>
         <v>8.0489999999999995</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -1925,11 +1924,11 @@
         <v>94</v>
       </c>
       <c r="E87" s="2">
-        <f>(B87*60)+C87+(D87/1000)</f>
+        <f t="shared" si="2"/>
         <v>8.0939999999999994</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -1941,11 +1940,11 @@
         <v>18</v>
       </c>
       <c r="E88" s="2">
-        <f>(B88*60)+C88+(D88/1000)</f>
+        <f t="shared" si="2"/>
         <v>7.0179999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -1957,11 +1956,11 @@
         <v>53</v>
       </c>
       <c r="E89" s="2">
-        <f>(B89*60)+C89+(D89/1000)</f>
+        <f t="shared" si="2"/>
         <v>32.052999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -1973,11 +1972,11 @@
         <v>65</v>
       </c>
       <c r="E90" s="2">
-        <f>(B90*60)+C90+(D90/1000)</f>
+        <f t="shared" si="2"/>
         <v>12.065</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -1989,11 +1988,11 @@
         <v>94</v>
       </c>
       <c r="E91" s="2">
-        <f>(B91*60)+C91+(D91/1000)</f>
+        <f t="shared" si="2"/>
         <v>13.093999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2007,11 +2006,11 @@
         <v>60</v>
       </c>
       <c r="E92" s="2">
-        <f>(B92*60)+C92+(D92/1000)</f>
+        <f t="shared" si="2"/>
         <v>79.06</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2025,11 +2024,11 @@
         <v>93</v>
       </c>
       <c r="E93" s="2">
-        <f>(B93*60)+C93+(D93/1000)</f>
+        <f t="shared" si="2"/>
         <v>92.093000000000004</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2041,11 +2040,11 @@
         <v>67</v>
       </c>
       <c r="E94" s="2">
-        <f>(B94*60)+C94+(D94/1000)</f>
+        <f t="shared" si="2"/>
         <v>56.067</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2057,11 +2056,11 @@
         <v>70</v>
       </c>
       <c r="E95" s="2">
-        <f>(B95*60)+C95+(D95/1000)</f>
+        <f t="shared" si="2"/>
         <v>9.07</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2073,11 +2072,11 @@
         <v>83</v>
       </c>
       <c r="E96" s="2">
-        <f>(B96*60)+C96+(D96/1000)</f>
+        <f t="shared" si="2"/>
         <v>24.082999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2091,11 +2090,11 @@
         <v>94</v>
       </c>
       <c r="E97" s="2">
-        <f>(B97*60)+C97+(D97/1000)</f>
+        <f t="shared" si="2"/>
         <v>83.093999999999994</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2107,11 +2106,11 @@
         <v>82</v>
       </c>
       <c r="E98" s="2">
-        <f>(B98*60)+C98+(D98/1000)</f>
+        <f t="shared" ref="E98:E129" si="3">(B98*60)+C98+(D98/1000)</f>
         <v>22.082000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2123,11 +2122,11 @@
         <v>48</v>
       </c>
       <c r="E99" s="2">
-        <f>(B99*60)+C99+(D99/1000)</f>
+        <f t="shared" si="3"/>
         <v>38.048000000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2141,11 +2140,11 @@
         <v>59</v>
       </c>
       <c r="E100" s="2">
-        <f>(B100*60)+C100+(D100/1000)</f>
+        <f t="shared" si="3"/>
         <v>89.058999999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2157,11 +2156,11 @@
         <v>50</v>
       </c>
       <c r="E101" s="2">
-        <f>(B101*60)+C101+(D101/1000)</f>
+        <f t="shared" si="3"/>
         <v>17.05</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2173,11 +2172,11 @@
         <v>16</v>
       </c>
       <c r="E102" s="2">
-        <f>(B102*60)+C102+(D102/1000)</f>
+        <f t="shared" si="3"/>
         <v>11.016</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2189,11 +2188,11 @@
         <v>84</v>
       </c>
       <c r="E103" s="2">
-        <f>(B103*60)+C103+(D103/1000)</f>
+        <f t="shared" si="3"/>
         <v>35.084000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2207,11 +2206,11 @@
         <v>21</v>
       </c>
       <c r="E104" s="2">
-        <f>(B104*60)+C104+(D104/1000)</f>
+        <f t="shared" si="3"/>
         <v>66.021000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2223,11 +2222,11 @@
         <v>85</v>
       </c>
       <c r="E105" s="2">
-        <f>(B105*60)+C105+(D105/1000)</f>
+        <f t="shared" si="3"/>
         <v>13.085000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2241,11 +2240,11 @@
         <v>46</v>
       </c>
       <c r="E106" s="2">
-        <f>(B106*60)+C106+(D106/1000)</f>
+        <f t="shared" si="3"/>
         <v>70.046000000000006</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2257,11 +2256,11 @@
         <v>68</v>
       </c>
       <c r="E107" s="2">
-        <f>(B107*60)+C107+(D107/1000)</f>
+        <f t="shared" si="3"/>
         <v>22.068000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2273,11 +2272,11 @@
         <v>35</v>
       </c>
       <c r="E108" s="2">
-        <f>(B108*60)+C108+(D108/1000)</f>
+        <f t="shared" si="3"/>
         <v>42.034999999999997</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2291,11 +2290,11 @@
         <v>78</v>
       </c>
       <c r="E109" s="2">
-        <f>(B109*60)+C109+(D109/1000)</f>
+        <f t="shared" si="3"/>
         <v>74.078000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2307,11 +2306,11 @@
         <v>67</v>
       </c>
       <c r="E110" s="2">
-        <f>(B110*60)+C110+(D110/1000)</f>
+        <f t="shared" si="3"/>
         <v>10.067</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2325,11 +2324,11 @@
         <v>38</v>
       </c>
       <c r="E111" s="2">
-        <f>(B111*60)+C111+(D111/1000)</f>
+        <f t="shared" si="3"/>
         <v>67.037999999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2343,11 +2342,11 @@
         <v>61</v>
       </c>
       <c r="E112" s="2">
-        <f>(B112*60)+C112+(D112/1000)</f>
+        <f t="shared" si="3"/>
         <v>92.061000000000007</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2361,11 +2360,11 @@
         <v>54</v>
       </c>
       <c r="E113" s="2">
-        <f>(B113*60)+C113+(D113/1000)</f>
+        <f t="shared" si="3"/>
         <v>71.054000000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2377,11 +2376,11 @@
         <v>31</v>
       </c>
       <c r="E114" s="2">
-        <f>(B114*60)+C114+(D114/1000)</f>
+        <f t="shared" si="3"/>
         <v>25.030999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2393,11 +2392,11 @@
         <v>47</v>
       </c>
       <c r="E115" s="2">
-        <f>(B115*60)+C115+(D115/1000)</f>
+        <f t="shared" si="3"/>
         <v>16.047000000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2409,11 +2408,11 @@
         <v>91</v>
       </c>
       <c r="E116" s="2">
-        <f>(B116*60)+C116+(D116/1000)</f>
+        <f t="shared" si="3"/>
         <v>38.091000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2427,11 +2426,11 @@
         <v>80</v>
       </c>
       <c r="E117" s="2">
-        <f>(B117*60)+C117+(D117/1000)</f>
+        <f t="shared" si="3"/>
         <v>78.08</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2445,11 +2444,11 @@
         <v>57</v>
       </c>
       <c r="E118" s="2">
-        <f>(B118*60)+C118+(D118/1000)</f>
+        <f t="shared" si="3"/>
         <v>123.057</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2461,11 +2460,11 @@
         <v>59</v>
       </c>
       <c r="E119" s="2">
-        <f>(B119*60)+C119+(D119/1000)</f>
+        <f t="shared" si="3"/>
         <v>11.058999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2477,11 +2476,11 @@
         <v>9</v>
       </c>
       <c r="E120" s="2">
-        <f>(B120*60)+C120+(D120/1000)</f>
+        <f t="shared" si="3"/>
         <v>17.009</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2493,11 +2492,11 @@
         <v>64</v>
       </c>
       <c r="E121" s="2">
-        <f>(B121*60)+C121+(D121/1000)</f>
+        <f t="shared" si="3"/>
         <v>35.064</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2509,11 +2508,11 @@
         <v>84</v>
       </c>
       <c r="E122" s="2">
-        <f>(B122*60)+C122+(D122/1000)</f>
+        <f t="shared" si="3"/>
         <v>27.084</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2525,11 +2524,11 @@
         <v>3</v>
       </c>
       <c r="E123" s="2">
-        <f>(B123*60)+C123+(D123/1000)</f>
+        <f t="shared" si="3"/>
         <v>16.003</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2541,11 +2540,11 @@
         <v>83</v>
       </c>
       <c r="E124" s="2">
-        <f>(B124*60)+C124+(D124/1000)</f>
+        <f t="shared" si="3"/>
         <v>12.083</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2557,11 +2556,11 @@
         <v>32</v>
       </c>
       <c r="E125" s="2">
-        <f>(B125*60)+C125+(D125/1000)</f>
+        <f t="shared" si="3"/>
         <v>49.031999999999996</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -2573,11 +2572,11 @@
         <v>68</v>
       </c>
       <c r="E126" s="2">
-        <f>(B126*60)+C126+(D126/1000)</f>
+        <f t="shared" si="3"/>
         <v>42.067999999999998</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -2589,11 +2588,11 @@
         <v>80</v>
       </c>
       <c r="E127" s="2">
-        <f>(B127*60)+C127+(D127/1000)</f>
+        <f t="shared" si="3"/>
         <v>32.08</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -2605,11 +2604,11 @@
         <v>26</v>
       </c>
       <c r="E128" s="2">
-        <f>(B128*60)+C128+(D128/1000)</f>
+        <f t="shared" si="3"/>
         <v>7.0259999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -2621,11 +2620,11 @@
         <v>27</v>
       </c>
       <c r="E129" s="2">
-        <f>(B129*60)+C129+(D129/1000)</f>
+        <f t="shared" si="3"/>
         <v>46.027000000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -2637,11 +2636,11 @@
         <v>41</v>
       </c>
       <c r="E130" s="2">
-        <f>(B130*60)+C130+(D130/1000)</f>
+        <f t="shared" ref="E130:E168" si="4">(B130*60)+C130+(D130/1000)</f>
         <v>18.041</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -2653,11 +2652,11 @@
         <v>46</v>
       </c>
       <c r="E131" s="2">
-        <f>(B131*60)+C131+(D131/1000)</f>
+        <f t="shared" si="4"/>
         <v>43.045999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -2669,11 +2668,11 @@
         <v>3</v>
       </c>
       <c r="E132" s="2">
-        <f>(B132*60)+C132+(D132/1000)</f>
+        <f t="shared" si="4"/>
         <v>32.003</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -2685,11 +2684,11 @@
         <v>60</v>
       </c>
       <c r="E133" s="2">
-        <f>(B133*60)+C133+(D133/1000)</f>
+        <f t="shared" si="4"/>
         <v>8.06</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -2701,11 +2700,11 @@
         <v>18</v>
       </c>
       <c r="E134" s="2">
-        <f>(B134*60)+C134+(D134/1000)</f>
+        <f t="shared" si="4"/>
         <v>26.018000000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -2717,11 +2716,11 @@
         <v>26</v>
       </c>
       <c r="E135" s="2">
-        <f>(B135*60)+C135+(D135/1000)</f>
+        <f t="shared" si="4"/>
         <v>7.0259999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -2733,11 +2732,11 @@
         <v>58</v>
       </c>
       <c r="E136" s="2">
-        <f>(B136*60)+C136+(D136/1000)</f>
+        <f t="shared" si="4"/>
         <v>6.0579999999999998</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -2749,11 +2748,11 @@
         <v>81</v>
       </c>
       <c r="E137" s="2">
-        <f>(B137*60)+C137+(D137/1000)</f>
+        <f t="shared" si="4"/>
         <v>10.081</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -2765,11 +2764,11 @@
         <v>23</v>
       </c>
       <c r="E138" s="2">
-        <f>(B138*60)+C138+(D138/1000)</f>
+        <f t="shared" si="4"/>
         <v>38.023000000000003</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -2781,11 +2780,11 @@
         <v>20</v>
       </c>
       <c r="E139" s="2">
-        <f>(B139*60)+C139+(D139/1000)</f>
+        <f t="shared" si="4"/>
         <v>21.02</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -2797,11 +2796,11 @@
         <v>95</v>
       </c>
       <c r="E140" s="2">
-        <f>(B140*60)+C140+(D140/1000)</f>
+        <f t="shared" si="4"/>
         <v>30.094999999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -2813,11 +2812,11 @@
         <v>30</v>
       </c>
       <c r="E141" s="2">
-        <f>(B141*60)+C141+(D141/1000)</f>
+        <f t="shared" si="4"/>
         <v>19.03</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -2831,11 +2830,11 @@
         <v>77</v>
       </c>
       <c r="E142" s="2">
-        <f>(B142*60)+C142+(D142/1000)</f>
+        <f t="shared" si="4"/>
         <v>93.076999999999998</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -2847,11 +2846,11 @@
         <v>0</v>
       </c>
       <c r="E143" s="2">
-        <f>(B143*60)+C143+(D143/1000)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -2863,11 +2862,11 @@
         <v>91</v>
       </c>
       <c r="E144" s="2">
-        <f>(B144*60)+C144+(D144/1000)</f>
+        <f t="shared" si="4"/>
         <v>29.091000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -2879,11 +2878,11 @@
         <v>11</v>
       </c>
       <c r="E145" s="2">
-        <f>(B145*60)+C145+(D145/1000)</f>
+        <f t="shared" si="4"/>
         <v>8.0109999999999992</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -2895,11 +2894,11 @@
         <v>90</v>
       </c>
       <c r="E146" s="2">
-        <f>(B146*60)+C146+(D146/1000)</f>
+        <f t="shared" si="4"/>
         <v>29.09</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -2913,11 +2912,11 @@
         <v>17</v>
       </c>
       <c r="E147" s="2">
-        <f>(B147*60)+C147+(D147/1000)</f>
+        <f t="shared" si="4"/>
         <v>90.016999999999996</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -2929,11 +2928,11 @@
         <v>39</v>
       </c>
       <c r="E148" s="2">
-        <f>(B148*60)+C148+(D148/1000)</f>
+        <f t="shared" si="4"/>
         <v>17.039000000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -2945,11 +2944,11 @@
         <v>42</v>
       </c>
       <c r="E149" s="2">
-        <f>(B149*60)+C149+(D149/1000)</f>
+        <f t="shared" si="4"/>
         <v>33.042000000000002</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -2963,11 +2962,11 @@
         <v>55</v>
       </c>
       <c r="E150" s="2">
-        <f>(B150*60)+C150+(D150/1000)</f>
+        <f t="shared" si="4"/>
         <v>133.05500000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -2981,11 +2980,11 @@
         <v>23</v>
       </c>
       <c r="E151" s="2">
-        <f>(B151*60)+C151+(D151/1000)</f>
+        <f t="shared" si="4"/>
         <v>79.022999999999996</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -2997,11 +2996,11 @@
         <v>55</v>
       </c>
       <c r="E152" s="2">
-        <f>(B152*60)+C152+(D152/1000)</f>
+        <f t="shared" si="4"/>
         <v>32.055</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -3013,11 +3012,11 @@
         <v>51</v>
       </c>
       <c r="E153" s="2">
-        <f>(B153*60)+C153+(D153/1000)</f>
+        <f t="shared" si="4"/>
         <v>17.050999999999998</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>6</v>
       </c>
       <c r="E154" s="2">
-        <f>(B154*60)+C154+(D154/1000)</f>
+        <f t="shared" si="4"/>
         <v>14.006</v>
       </c>
     </row>
@@ -3038,126 +3037,232 @@
         <v>154</v>
       </c>
       <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="3"/>
+      <c r="C155" s="3">
+        <v>19</v>
+      </c>
+      <c r="D155" s="3">
+        <v>41</v>
+      </c>
+      <c r="E155" s="3">
+        <f t="shared" si="4"/>
+        <v>19.041</v>
+      </c>
     </row>
     <row r="156" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>155</v>
       </c>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
+      <c r="B156" s="3">
+        <v>1</v>
+      </c>
+      <c r="C156" s="3">
+        <v>27</v>
+      </c>
+      <c r="D156" s="3">
+        <v>7</v>
+      </c>
+      <c r="E156" s="2">
+        <f t="shared" si="4"/>
+        <v>87.007000000000005</v>
+      </c>
     </row>
     <row r="157" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>156</v>
       </c>
       <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
+      <c r="C157" s="3">
+        <v>24</v>
+      </c>
+      <c r="D157" s="3">
+        <v>29</v>
+      </c>
+      <c r="E157" s="3">
+        <f t="shared" si="4"/>
+        <v>24.029</v>
+      </c>
     </row>
     <row r="158" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>157</v>
       </c>
       <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
+      <c r="C158" s="3">
+        <v>11</v>
+      </c>
+      <c r="D158" s="3">
+        <v>43</v>
+      </c>
+      <c r="E158" s="2">
+        <f t="shared" si="4"/>
+        <v>11.042999999999999</v>
+      </c>
     </row>
     <row r="159" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>158</v>
       </c>
       <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
-      <c r="E159" s="3"/>
+      <c r="C159" s="3">
+        <v>31</v>
+      </c>
+      <c r="D159" s="3">
+        <v>1</v>
+      </c>
+      <c r="E159" s="3">
+        <f t="shared" si="4"/>
+        <v>31.001000000000001</v>
+      </c>
     </row>
     <row r="160" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>159</v>
       </c>
       <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="3"/>
+      <c r="C160" s="3">
+        <v>42</v>
+      </c>
+      <c r="D160" s="3">
+        <v>73</v>
+      </c>
+      <c r="E160" s="2">
+        <f t="shared" si="4"/>
+        <v>42.073</v>
+      </c>
     </row>
     <row r="161" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>160</v>
       </c>
       <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
+      <c r="C161" s="3">
+        <v>4</v>
+      </c>
+      <c r="D161" s="3">
+        <v>42</v>
+      </c>
+      <c r="E161" s="3">
+        <f t="shared" si="4"/>
+        <v>4.0419999999999998</v>
+      </c>
     </row>
     <row r="162" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>161</v>
       </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
+      <c r="B162" s="3">
+        <v>1</v>
+      </c>
+      <c r="C162" s="3">
+        <v>5</v>
+      </c>
+      <c r="D162" s="3">
+        <v>91</v>
+      </c>
+      <c r="E162" s="2">
+        <f t="shared" si="4"/>
+        <v>65.090999999999994</v>
+      </c>
     </row>
     <row r="163" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>162</v>
       </c>
       <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
+      <c r="C163" s="3">
+        <v>34</v>
+      </c>
+      <c r="D163" s="3">
+        <v>23</v>
+      </c>
+      <c r="E163" s="3">
+        <f t="shared" si="4"/>
+        <v>34.023000000000003</v>
+      </c>
     </row>
     <row r="164" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>163</v>
       </c>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
+      <c r="B164" s="3">
+        <v>1</v>
+      </c>
+      <c r="C164" s="3">
+        <v>3</v>
+      </c>
+      <c r="D164" s="3">
+        <v>45</v>
+      </c>
+      <c r="E164" s="2">
+        <f t="shared" si="4"/>
+        <v>63.045000000000002</v>
+      </c>
     </row>
     <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>164</v>
       </c>
       <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="3"/>
+      <c r="C165" s="3">
+        <v>26</v>
+      </c>
+      <c r="D165" s="3">
+        <v>56</v>
+      </c>
+      <c r="E165" s="3">
+        <f t="shared" si="4"/>
+        <v>26.056000000000001</v>
+      </c>
     </row>
     <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>165</v>
       </c>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
-      <c r="E166" s="3"/>
+      <c r="B166" s="3">
+        <v>1</v>
+      </c>
+      <c r="C166" s="3">
+        <v>5</v>
+      </c>
+      <c r="D166" s="3">
+        <v>91</v>
+      </c>
+      <c r="E166" s="2">
+        <f t="shared" si="4"/>
+        <v>65.090999999999994</v>
+      </c>
     </row>
     <row r="167" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>166</v>
       </c>
       <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="3"/>
+      <c r="C167" s="3">
+        <v>20</v>
+      </c>
+      <c r="D167" s="3">
+        <v>87</v>
+      </c>
+      <c r="E167" s="3">
+        <f t="shared" si="4"/>
+        <v>20.087</v>
+      </c>
     </row>
     <row r="168" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>167</v>
       </c>
       <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
-      <c r="E168" s="3"/>
+      <c r="C168" s="3">
+        <v>12</v>
+      </c>
+      <c r="D168" s="3">
+        <v>78</v>
+      </c>
+      <c r="E168" s="2">
+        <f t="shared" si="4"/>
+        <v>12.077999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3171,7 +3276,7 @@
   </sheetPr>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3184,31 +3289,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3264,7 +3369,7 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f>((1.96^2)*(G2^2))/(5^2)</f>
         <v>86.895338617043222</v>
       </c>
@@ -5048,10 +5153,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5063,31 +5168,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5105,7 +5210,7 @@
         <v>84</v>
       </c>
       <c r="E2" s="6">
-        <f t="shared" ref="E2:E118" si="0">(B2*60)+C2+(D2/1000)</f>
+        <f t="shared" ref="E2:E116" si="0">(B2*60)+C2+(D2/1000)</f>
         <v>20.084</v>
       </c>
       <c r="F2" s="6">
@@ -5141,7 +5246,7 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <f>((1.96^2)*(G2^2))/(1^2)</f>
         <v>341.28387032484773</v>
       </c>
@@ -6968,33 +7073,289 @@
       <c r="A117" s="2">
         <v>116</v>
       </c>
-      <c r="B117" s="3"/>
-      <c r="C117" s="2">
-        <v>20</v>
-      </c>
-      <c r="D117" s="2">
-        <v>82</v>
-      </c>
-      <c r="E117" s="2">
-        <f t="shared" si="0"/>
-        <v>20.082000000000001</v>
-      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
       <c r="B118" s="3"/>
-      <c r="C118" s="2">
-        <v>16</v>
-      </c>
-      <c r="D118" s="2">
-        <v>69</v>
-      </c>
-      <c r="E118" s="2">
-        <f t="shared" si="0"/>
-        <v>16.068999999999999</v>
-      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+    </row>
+    <row r="142" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+    </row>
+    <row r="144" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+    </row>
+    <row r="145" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+    </row>
+    <row r="146" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+    </row>
+    <row r="148" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7006,10 +7367,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7021,31 +7382,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
@@ -8698,6 +9059,348 @@
         <f t="shared" si="0"/>
         <v>51.003999999999998</v>
       </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+    </row>
+    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+    </row>
+    <row r="134" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8711,8 +9414,8 @@
   </sheetPr>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8723,36 +9426,36 @@
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -8764,7 +9467,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="6">
-        <f t="shared" ref="E2:E55" si="0">(B2*60)+C2+(D2/1000)</f>
+        <f t="shared" ref="E2:E65" si="0">(B2*60)+C2+(D2/1000)</f>
         <v>29.082999999999998</v>
       </c>
       <c r="F2" s="8">
@@ -8783,7 +9486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -8799,7 +9502,7 @@
         <v>17.030999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -8816,7 +9519,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -8832,7 +9535,7 @@
         <v>20.068000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -8848,7 +9551,7 @@
         <v>12.048</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -8865,7 +9568,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -8881,7 +9584,7 @@
         <v>59.094000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -8898,7 +9601,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -8914,7 +9617,7 @@
         <v>25.004000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -8930,7 +9633,7 @@
         <v>27.077000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -8946,7 +9649,7 @@
         <v>24.032</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -8962,7 +9665,7 @@
         <v>27.077999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -8978,7 +9681,7 @@
         <v>54.091000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -8994,7 +9697,7 @@
         <v>48.033000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -9010,7 +9713,7 @@
         <v>45.097999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -9026,7 +9729,7 @@
         <v>32.012999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -9042,7 +9745,7 @@
         <v>14.036</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -9058,7 +9761,7 @@
         <v>43.029000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -9074,7 +9777,7 @@
         <v>33.042999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -9090,7 +9793,7 @@
         <v>24.009</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -9106,7 +9809,7 @@
         <v>49.076999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -9122,7 +9825,7 @@
         <v>50.006</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -9138,7 +9841,7 @@
         <v>46.054000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -9154,7 +9857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -9170,7 +9873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -9186,7 +9889,7 @@
         <v>22.076000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -9202,7 +9905,7 @@
         <v>35.046999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -9218,7 +9921,7 @@
         <v>41.027999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -9234,7 +9937,7 @@
         <v>26.085000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -9250,7 +9953,7 @@
         <v>36.088999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -9266,7 +9969,7 @@
         <v>32.069000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -9284,7 +9987,7 @@
         <v>66.052999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -9302,7 +10005,7 @@
         <v>79.075999999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -9318,7 +10021,7 @@
         <v>23.068999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -9336,7 +10039,7 @@
         <v>80.001000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -9354,7 +10057,7 @@
         <v>76.075000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -9370,7 +10073,7 @@
         <v>7.03</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -9386,7 +10089,7 @@
         <v>33.008000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -9402,7 +10105,7 @@
         <v>47.085999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -9418,7 +10121,7 @@
         <v>42.033999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -9434,7 +10137,7 @@
         <v>45.027000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -9450,7 +10153,7 @@
         <v>16.045000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -9466,7 +10169,7 @@
         <v>21.076000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -9482,7 +10185,7 @@
         <v>27.065999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -9500,7 +10203,7 @@
         <v>63.012</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -9518,7 +10221,7 @@
         <v>72.007000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -9534,7 +10237,7 @@
         <v>37.017000000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -9550,7 +10253,7 @@
         <v>47.037999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -9566,7 +10269,7 @@
         <v>19.052</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -9582,7 +10285,7 @@
         <v>9.077</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -9598,7 +10301,7 @@
         <v>43.066000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -9614,7 +10317,7 @@
         <v>24.084</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -9630,7 +10333,7 @@
         <v>11.009</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -9651,117 +10354,212 @@
         <v>55</v>
       </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="C56" s="3">
+        <v>15</v>
+      </c>
+      <c r="D56" s="3">
+        <v>24</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="0"/>
+        <v>15.023999999999999</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="C57" s="3">
+        <v>45</v>
+      </c>
+      <c r="D57" s="3">
+        <v>77</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="0"/>
+        <v>45.076999999999998</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
+      <c r="C58" s="3">
+        <v>21</v>
+      </c>
+      <c r="D58" s="3">
+        <v>85</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="0"/>
+        <v>21.085000000000001</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+      <c r="B59" s="3">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3">
+        <v>8</v>
+      </c>
+      <c r="D59" s="3">
+        <v>32</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="0"/>
+        <v>128.03200000000001</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
+      <c r="C60" s="3">
+        <v>50</v>
+      </c>
+      <c r="D60" s="3">
+        <v>88</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="0"/>
+        <v>50.088000000000001</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="C61" s="3">
+        <v>26</v>
+      </c>
+      <c r="D61" s="3">
+        <v>84</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="0"/>
+        <v>26.084</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
+      <c r="C62" s="3">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3">
+        <v>95</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="0"/>
+        <v>17.094999999999999</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
+      <c r="C63" s="3">
+        <v>34</v>
+      </c>
+      <c r="D63" s="3">
+        <v>36</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="0"/>
+        <v>34.036000000000001</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
+      <c r="C64" s="3">
+        <v>12</v>
+      </c>
+      <c r="D64" s="3">
+        <v>18</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="0"/>
+        <v>12.018000000000001</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3">
+        <v>23</v>
+      </c>
+      <c r="D65" s="3">
+        <v>93</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="0"/>
+        <v>83.093000000000004</v>
+      </c>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
+      <c r="C66" s="3">
+        <v>23</v>
+      </c>
+      <c r="D66" s="3">
+        <v>82</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" ref="E66:E68" si="1">(B66*60)+C66+(D66/1000)</f>
+        <v>23.082000000000001</v>
+      </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
       <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
+      <c r="C67" s="3">
+        <v>31</v>
+      </c>
+      <c r="D67" s="3">
+        <v>44</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="1"/>
+        <v>31.044</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
+      <c r="C68" s="3">
+        <v>18</v>
+      </c>
+      <c r="D68" s="3">
+        <v>25</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="1"/>
+        <v>18.024999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>